<commit_message>
creates hash table from testlistworksheet
</commit_message>
<xml_diff>
--- a/ZephyrScaleTraceabilityMatrixReport/ZephyrScaleTraceabilityMatrixReport/Reports/Output.xlsx
+++ b/ZephyrScaleTraceabilityMatrixReport/ZephyrScaleTraceabilityMatrixReport/Reports/Output.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\zephyr-reports\ZephyrScaleTraceabilityMatrixReport\ZephyrScaleTraceabilityMatrixReport\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00178B7-7CCD-4949-8BA9-10F4697CE991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE834F1-90DD-4A2D-93AB-84C9D7F21D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31665" yWindow="1590" windowWidth="21600" windowHeight="11505" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCoverageMatrix" sheetId="1" r:id="rId1"/>
     <sheet name="TestCaseList" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>hello world</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>CMW-T1</t>
   </si>
@@ -77,8 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,17 +83,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF008000" tint="0"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -112,9 +103,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,64 +422,60 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
@@ -501,57 +487,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fills out traceability matrix
</commit_message>
<xml_diff>
--- a/ZephyrScaleTraceabilityMatrixReport/ZephyrScaleTraceabilityMatrixReport/Reports/Output.xlsx
+++ b/ZephyrScaleTraceabilityMatrixReport/ZephyrScaleTraceabilityMatrixReport/Reports/Output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\zephyr-reports\ZephyrScaleTraceabilityMatrixReport\ZephyrScaleTraceabilityMatrixReport\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE834F1-90DD-4A2D-93AB-84C9D7F21D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC5DA6C-FFF3-4E5F-913E-72A21564C4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CMW-T1</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>AUTO-1</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
   <si>
     <t>AUTO-3</t>
@@ -423,7 +426,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,30 +452,54 @@
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -505,10 +532,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -516,10 +543,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -527,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -535,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>